<commit_message>
fix bugs add new charts
</commit_message>
<xml_diff>
--- a/src/output/3-filter/manual/all-nf.xlsx
+++ b/src/output/3-filter/manual/all-nf.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>privacy,operate system security,nothing</t>
+          <t>nothing,privacy,operate system security</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>digital cash,electronic commerce,apply compute</t>
+          <t>electronic commerce,apply compute,digital cash</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>extra-functional property,compute platform,software performance,privacy,it engineer,information system application,software organization,property,nothing,information system</t>
+          <t>software performance,privacy,nothing,property,extra-functional property,compute platform,software organization,information system application,information system,it engineer</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -640,7 +640,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -687,7 +687,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ethereum,overflow vulnerability,taint analysis,contract</t>
+          <t>overflow vulnerability,contract,ethereum,taint analysis</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -734,7 +734,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>network simulation,privacy,network,network performance evaluation,nothing</t>
+          <t>network performance evaluation,network,privacy,nothing,network simulation</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -828,7 +828,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>privacy,database,storage security,nothing</t>
+          <t>nothing,database,storage security,privacy</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>wide,privacy,web mine,web,malware mitigation,web application security,nothing,intrusion/anomaly detection,world,information system</t>
+          <t>malware mitigation,world,wide,privacy,web,nothing,web mine,web application security,information system,intrusion/anomaly detection</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -922,7 +922,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -969,7 +969,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>social,apply compute,privacy,online bank,professional topic,compute,secure online transaction,nothing,privacy policy,electronic fund transfer,technology policy,domain-specific security and privacy architecture,electronic commerce</t>
+          <t>privacy policy,compute,privacy,social,secure online transaction,professional topic,nothing,apply compute,electronic fund transfer,domain-specific security and privacy architecture,technology policy,electronic commerce,online bank</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>privacy,authentication,security service,nothing,multi-factor authentication</t>
+          <t>privacy,nothing,authentication,multi-factor authentication,security service</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>program,program language usability,nothing</t>
+          <t>nothing,program language usability,program</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>tool,privacy,software library,it engineer,repository,nothing,software notation</t>
+          <t>software notation,software library,privacy,tool,nothing,repository,it engineer</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>privacy,professional topic,compute,privacy policy,nothing,technology policy,social</t>
+          <t>privacy policy,compute,professional topic,privacy,social,nothing,technology policy</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>software verification,software defect analysis,privacy,it engineer,management,software test,validation,debug,nothing,software creation</t>
+          <t>privacy,management,software verification,nothing,debug,software creation,software defect analysis,software test,validation,it engineer</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>security protocol,privacy,network,nothing,network architecture</t>
+          <t>network,privacy,nothing,security protocol,network architecture</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>privacy,domain-specific security and privacy architecture,nothing</t>
+          <t>nothing,domain-specific security and privacy architecture,privacy</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>distribute architecture,network,denial-of-service attack,nothing,peer-to-peer architecture,computer system organization</t>
+          <t>network,nothing,peer-to-peer architecture,denial-of-service attack,distribute architecture,computer system organization</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>time-based model,attacker advantage,mathematical model,bitcoin,double-spend attack</t>
+          <t>double-spend attack,bitcoin,mathematical model,attacker advantage,time-based model</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>privacy,message authentication code,symmetric cryptography,nothing,cryptography</t>
+          <t>cryptography,privacy,nothing,symmetric cryptography,message authentication code</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>privacy,operate system security,nothing</t>
+          <t>nothing,privacy,operate system security</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>distribute denial-of-service ,cooperative defense,nothing</t>
+          <t xml:space="preserve">cooperative defense,nothing,distribute denial-of-service </t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1815,7 +1815,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>privacy,network,statistic,network protocol,mathematics of compute,nothing,probability,cryptography</t>
+          <t>cryptography,probability,network,privacy,nothing,network protocol,mathematics of compute,statistic</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>privacy,theory of security,nothing,logic,formal approach,security in hardware</t>
+          <t>privacy,nothing,formal approach,theory of security,security in hardware,logic</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>distribute architecture,network,network reliability,nothing,peer-to-peer architecture,computer system organization</t>
+          <t>network,nothing,peer-to-peer architecture,network reliability,distribute architecture,computer system organization</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -2097,7 +2097,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>security protocol,privacy,distribute architecture,network,wireless security,security service,nothing,peer-to-peer architecture,computer system organization,mobile,privacy-preserving protocol</t>
+          <t>network,privacy,wireless security,nothing,peer-to-peer architecture,security protocol,mobile,security service,distribute architecture,privacy-preserving protocol,computer system organization</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>digital cash,apply compute,privacy,nothing,electronic commerce</t>
+          <t>privacy,nothing,apply compute,digital cash,electronic commerce</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>privacy,cryptography,key management,nothing</t>
+          <t>cryptography,nothing,key management,privacy</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>privacy,network,nothing</t>
+          <t>nothing,network,privacy</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>document type,privacy,general conference proceed,nothing,general,reference</t>
+          <t>document type,privacy,nothing,reference,general conference proceed,general</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>database,privacy,query of encrypt data,management,storage security,nothing</t>
+          <t>database,storage security,privacy,management,nothing,query of encrypt data</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>privacy,authorization,security service,nothing</t>
+          <t>authorization,nothing,security service,privacy</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2520,7 +2520,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>privacy,theory of security,nothing,logic,formal approach</t>
+          <t>privacy,nothing,formal approach,theory of security,logic</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>privacy,domain-specific security and privacy architecture,nothing</t>
+          <t>nothing,domain-specific security and privacy architecture,privacy</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2614,7 +2614,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>page strategy,record storage system,information storage system,block,information system</t>
+          <t>page strategy,information storage system,record storage system,block,information system</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>domain specific language,formal approach,security evaluation,nothing</t>
+          <t>nothing,domain specific language,formal approach,security evaluation</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>privacy,professional topic,compute,privacy policy,nothing,technology policy,social</t>
+          <t>privacy policy,compute,professional topic,privacy,social,nothing,technology policy</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>privacy,message authentication code,symmetric cryptography,nothing,cryptography</t>
+          <t>cryptography,privacy,nothing,symmetric cryptography,message authentication code</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>privacy,database,storage security,nothing</t>
+          <t>nothing,database,storage security,privacy</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>privacy,network,network reliability,nothing</t>
+          <t>network reliability,nothing,network,privacy</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>unsupervised learn,anomaly detection,privacy,supervise learn,compute methodology,nothing,learn paradigm,machine learning</t>
+          <t>privacy,unsupervised learn,nothing,compute methodology,machine learning,learn paradigm,supervise learn,anomaly detection</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>network,denial-of-service attack,nothing</t>
+          <t>nothing,denial-of-service attack,network</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -3084,7 +3084,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>anonymity,theory of computation,cryptographic protocol,privacy,untraceability,nothing,security service,cryptography,privacy-preserving protocol,pseudonymity,computational complexity</t>
+          <t>theory of computation,cryptography,privacy,pseudonymity,nothing,computational complexity,anonymity,security service,cryptographic protocol,privacy-preserving protocol,untraceability</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -3131,7 +3131,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>hyperledger fabric,post-quantum cryptography,nothing</t>
+          <t>nothing,hyperledger fabric,post-quantum cryptography</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>privacy,nothing,internet of things,contract,consensus protocol</t>
+          <t>privacy,nothing,contract,consensus protocol,internet of things</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>general-purpose model,isolation,software bug,fault tolerance,autonomous robot,fault detection,internet of things,distribute compute,nothing,interaction,edge compute,computation</t>
+          <t>general-purpose model,edge compute,nothing,fault tolerance,distribute compute,computation,software bug,interaction,internet of things,isolation,fault detection,autonomous robot</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -3268,7 +3268,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>stateless protocol,genesis,bitcoin,digital linear tape,byzantine fault tolerance</t>
+          <t>stateless protocol,bitcoin,digital linear tape,byzantine fault tolerance,genesis</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>transfer function,program language,solidity,b-method,contract,first-order logic,immutable object,domain-specific language,nothing,principle of abstraction,first-order predicate,rodin tool,refinement ,validation,formal approach,type system,simulation,automate theorem prove,honeypot ,ethereum</t>
+          <t>first-order logic,domain-specific language,refinement ,simulation,type system,validation,principle of abstraction,contract,first-order predicate,program language,transfer function,solidity,automate theorem prove,nothing,ethereum,rodin tool,honeypot ,immutable object,formal approach,b-method</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -3362,7 +3362,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>immutable object,jot,sample ,malware,markov chain,double-spending,cryptocurrency,numerical analysis,iota,selection algorithm,adversary ,direct acyclic graph</t>
+          <t>adversary ,markov chain,double-spending,numerical analysis,cryptocurrency,sample ,direct acyclic graph,jot,malware,immutable object,selection algorithm,iota</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>throughput,commitment scheme,scalability,malware,amortize analysis,overhead ,shard ,recovery procedure,computation</t>
+          <t>throughput,shard ,scalability,malware,amortize analysis,overhead ,computation,commitment scheme,recovery procedure</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -3457,7 +3457,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>holographic principle,contract,information sensitivity,personally identifiable information,scalability,privacy,business logic,business process,entity,naruto shippuden: clash of ninja revolution 3,nothing,interaction,computation,enterprise system,confidentiality,enterprise integration,data integrity,spectral leakage,encryption</t>
+          <t>confidentiality,data integrity,enterprise system,interaction,scalability,information sensitivity,enterprise integration,holographic principle,naruto shippuden: clash of ninja revolution 3,business process,contract,privacy,nothing,computation,personally identifiable information,spectral leakage,encryption,business logic,entity</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>authorization,cryptographic hash function,network,tamper resistance,bitcoin,trust third party,differential privacy,pervasive informatics</t>
+          <t>cryptographic hash function,network,bitcoin,trust third party,differential privacy,tamper resistance,authorization,pervasive informatics</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -3551,7 +3551,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>database,computer,quantum entanglement,quantum algorithm,temporal logic,bitcoin,nothing,quantum compute,quantum information,ethereum,centralize compute</t>
+          <t>quantum entanglement,computer,database,temporal logic,quantum algorithm,nothing,bitcoin,quantum compute,ethereum,quantum information,centralize compute</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>value ,attack,social network,network,byzantine fault tolerance,proof-of-work system,web of trust</t>
+          <t>web of trust,attack,network,value ,byzantine fault tolerance,social network,proof-of-work system</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>immutable object,jot,procedural generation,simulation,mathematics,markov chain monte carlo,iota,selection algorithm,direct acyclic graph</t>
+          <t>procedural generation,jot,direct acyclic graph,mathematics,markov chain monte carlo,simulation,immutable object,selection algorithm,iota</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -3692,7 +3692,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>database,brute-force search,contract agreement,cryptocurrency,brute-force attack,bitcoin,antivirus software,marijuana abuse,contract,protocol documentation,cryptography</t>
+          <t>cryptography,database,contract agreement,cryptocurrency,bitcoin,marijuana abuse,antivirus software,contract,protocol documentation,brute-force attack,brute-force search</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>global network,essence,bitcoin,distribute compute,nothing</t>
+          <t>nothing,bitcoin,essence,distribute compute,global network</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3786,7 +3786,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>distribute transaction,cryptocurrency,bitcoin,internet of things,nothing,computation</t>
+          <t>cryptocurrency,bitcoin,nothing,distribute transaction,computation,internet of things</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>key derivation function,public-key cryptography,authorization,privacy,cryptonote,antivirus software,nothing,stealth,cryptography</t>
+          <t>cryptography,privacy,nothing,antivirus software,public-key cryptography,authorization,key derivation function,stealth,cryptonote</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -3880,7 +3880,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>lock ,business logic,computer data storage,computer performance,bitcoin,virtual machine,software portability,traction teampage,distribute compute,contract,nothing,ethereum,formal approach</t>
+          <t>software portability,lock ,traction teampage,nothing,bitcoin,ethereum,contract,formal approach,distribute compute,business logic,virtual machine,computer performance,computer data storage</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>asynchrony ,double-spending,shard ,replay attack</t>
+          <t>shard ,double-spending,asynchrony ,replay attack</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3974,7 +3974,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>sensor,public-key cryptography,population,bitcoin,internet of things,nothing,omness,home automation,machine learning</t>
+          <t>population,sensor,bitcoin,nothing,machine learning,omness,public-key cryptography,internet of things,home automation</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>rsa ,modulus robot,modulus of continuity,cryptography</t>
+          <t>rsa ,modulus robot,cryptography,modulus of continuity</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -4069,7 +4069,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>sensor,real-time clock,smart device,bitcoin,immutable object,ephrin type-b receptor 1,health fraud,cryptocurrency,entity,smartphone,program paradigm,tablet computer,exploit ,time complexity,e-commerce,human,smart city,exponential,tablet dosage form,solution,botnet,synergy,internet of things,certification</t>
+          <t>tablet dosage form,solution,cryptocurrency,e-commerce,smartphone,tablet computer,smart device,synergy,program paradigm,sensor,bitcoin,time complexity,human,real-time clock,internet of things,botnet,exploit ,ephrin type-b receptor 1,smart city,health fraud,immutable object,certification,entity,exponential</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -4116,7 +4116,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>immutable object,computer data storage,cryptocurrency,bitcoin,encryption,shamir's secret share,cryptography,zero-knowledge proof,identifier</t>
+          <t>cryptography,zero-knowledge proof,cryptocurrency,bitcoin,shamir's secret share,encryption,immutable object,computer data storage,identifier</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>mortar method,unintended consequence,moral hazard,contract,programmer</t>
+          <t>mortar method,unintended consequence,contract,moral hazard,programmer</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -4210,7 +4210,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>double-spending,cryptocurrency,bitcoin,node ,nothing,computational resource</t>
+          <t xml:space="preserve">double-spending,computational resource,nothing,bitcoin,cryptocurrency,node </t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>privacy,dust attack,cryptocurrency,bitcoin,nothing,threat</t>
+          <t>privacy,nothing,bitcoin,cryptocurrency,threat,dust attack</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>bitcoin,eclipse attack,countermeasure,peer-to-peer network,security analysis,block propagation</t>
+          <t>peer-to-peer network,eclipse attack,countermeasure,bitcoin,security analysis,block propagation</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -4351,7 +4351,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>decentralize payment system,p2p transaction,digital wallet,cryptocurrency,digital money,bitcoin,bitcoin security,bitcoin cyberattacks,nothing</t>
+          <t>p2p transaction,bitcoin cyberattacks,cryptocurrency,bitcoin,nothing,bitcoin security,digital wallet,digital money,decentralize payment system</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>bitcoin,internet of things,distribute system,nothing</t>
+          <t>nothing,bitcoin,internet of things,distribute system</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -4445,7 +4445,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>anomaly detection,nothing,machine learn ,bitcoin</t>
+          <t xml:space="preserve">nothing,bitcoin,anomaly detection,machine learn </t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -4492,7 +4492,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>conflict check protocol,attack,arbitration mechanism,conflict,bitcoin,nothing</t>
+          <t>attack,conflict,nothing,bitcoin,arbitration mechanism,conflict check protocol</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -4539,7 +4539,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>mine process,anonymity,decentralize,attack,bitcoin,miner,consensus protocol,block withhold</t>
+          <t>decentralize,attack,bitcoin,anonymity,miner,consensus protocol,block withhold,mine process</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -4586,7 +4586,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>attack,cryptocurrency exchange,bitcoin,cyber threat intelligence,nothing</t>
+          <t>cryptocurrency exchange,attack,nothing,bitcoin,cyber threat intelligence</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -4633,7 +4633,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>mine,attack,nothing</t>
+          <t>mine,nothing,attack</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -4680,7 +4680,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>light ethereum subprotocol,ethereum,light client,nothing</t>
+          <t>light ethereum subprotocol,nothing,ethereum,light client</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -4727,7 +4727,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>mine,attack,nothing</t>
+          <t>mine,nothing,attack</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -4774,7 +4774,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>hyper- ledger,attack,bitcoin,nothing,ethereum</t>
+          <t>attack,hyper- ledger,nothing,bitcoin,ethereum</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -4821,7 +4821,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>governance,nothing,software defect,hack,consensus protocol,cryptography,proof-of-stake</t>
+          <t>cryptography,governance,software defect,nothing,proof-of-stake,consensus protocol,hack</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -4868,7 +4868,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>blochchain,nothing,bitcoin</t>
+          <t>nothing,bitcoin,blochchain</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -4915,7 +4915,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>eclipse attack,nothing,network,bitcoin</t>
+          <t>nothing,bitcoin,eclipse attack,network</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -4962,7 +4962,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>attack surface,air gap storage,air gap wallet,key extraction,markov model,nothing,channel exfiltration,private key storage</t>
+          <t>attack surface,markov model,key extraction,air gap storage,nothing,private key storage,channel exfiltration,air gap wallet</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -5009,7 +5009,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>majority attack,nothing,proof of work ,bitcoin</t>
+          <t xml:space="preserve">nothing,bitcoin,majority attack,proof of work </t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -5056,7 +5056,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>bitcoin,dust attack,anti-dust,nothing</t>
+          <t>anti-dust,nothing,bitcoin,dust attack</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -5103,7 +5103,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>majority attack,network,anomaly detection,computer security,nothing,algorithmic game theory,machine learning</t>
+          <t>network,nothing,machine learning,computer security,algorithmic game theory,anomaly detection,majority attack</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>defence,vulnerability analysis,nothing,ethereum,geth</t>
+          <t>nothing,defence,ethereum,geth,vulnerability analysis</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -5197,7 +5197,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>double-spending,attack,bitcoin</t>
+          <t>attack,bitcoin,double-spending</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -5244,7 +5244,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>bitcoin,risk,contract,nothing,ethereum,threat</t>
+          <t>risk,nothing,bitcoin,ethereum,threat,contract</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -5291,7 +5291,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>nothing,countermeasure,objectionable content,bitcoin</t>
+          <t>countermeasure,nothing,bitcoin,objectionable content</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>nothing,database security,threat,bitcoin</t>
+          <t>bitcoin,nothing,database security,threat</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>privacy,hybrid,auction,nothing</t>
+          <t>nothing,auction,hybrid,privacy</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -5432,7 +5432,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>decentralization,network,cryptocurrency,bitcoin,internet of things,contract,nothing,survey</t>
+          <t>network,nothing,cryptocurrency,bitcoin,survey,contract,decentralization,internet of things</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -5479,7 +5479,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>trust,nothing</t>
+          <t>nothing,trust</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -5526,7 +5526,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>security practice,ibc,tendermint,nothing</t>
+          <t>tendermint,nothing,ibc,security practice</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -5573,7 +5573,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>nothing,contract theory,sharding,security deposit</t>
+          <t>sharding,nothing,security deposit,contract theory</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -5620,7 +5620,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>distribute trust,internet of things,on-off attack,nothing</t>
+          <t>distribute trust,nothing,internet of things,on-off attack</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -5667,7 +5667,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>commitment scheme,mine,selfish miner,block withhold attack,bitcoin mine</t>
+          <t>mine,selfish miner,block withhold attack,bitcoin mine,commitment scheme</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -5714,7 +5714,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>threat,cryptographic protocol,nothing</t>
+          <t>cryptographic protocol,nothing,threat</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -5761,7 +5761,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>mine,block withhold attack,fork after withhold</t>
+          <t>mine,fork after withhold,block withhold attack</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -5808,7 +5808,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>archival science,trust,bitcoin,secure compute,dependability,dependable,nothing</t>
+          <t>dependability,secure compute,nothing,bitcoin,trust,archival science,dependable</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -5855,7 +5855,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>storage balance,nothing</t>
+          <t>nothing,storage balance</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -5902,7 +5902,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>coin hop attack,pool mine,bitcoin,internet of things,nothing,ethereum</t>
+          <t>pool mine,nothing,bitcoin,ethereum,internet of things,coin hop attack</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -5949,7 +5949,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>uncle block,mine,eclipse attack,stubborn mine,ethereum</t>
+          <t>mine,eclipse attack,ethereum,stubborn mine,uncle block</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -5996,7 +5996,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>proof of authority,privacy,internet of thing ,nothing,ethereum</t>
+          <t>internet of thing ,privacy,nothing,ethereum,proof of authority</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -6043,7 +6043,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>threat categorization,threat,nothing</t>
+          <t>threat categorization,nothing,threat</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -6090,7 +6090,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>privacy,transaction system,nothing</t>
+          <t>transaction system,nothing,privacy</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>attack,delay attack,byzantine general problem,nothing,cryptography,partition</t>
+          <t>cryptography,attack,nothing,byzantine general problem,delay attack,partition</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -6184,7 +6184,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>risk,e-voting system,nothing</t>
+          <t>nothing,e-voting system,risk</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -6231,7 +6231,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>ethereum,man in the middle,nothing</t>
+          <t>man in the middle,nothing,ethereum</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -6278,7 +6278,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>ethereum,overflow vulnerability,taint analysis,contract</t>
+          <t>overflow vulnerability,contract,ethereum,taint analysis</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -6325,7 +6325,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>security vulnerability,atomicity violation,fuzzer,gas consumption,software test,vulnerability trigger,fuzzing,contract,nothing,ethereum</t>
+          <t>nothing,vulnerability trigger,ethereum,fuzzing,gas consumption,security vulnerability,atomicity violation,contract,software test,fuzzer</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -6372,7 +6372,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t xml:space="preserve">mine,bitcoin,block withhold attack,economics of mine,nothing,proof of work </t>
+          <t>mine,nothing,bitcoin,economics of mine,proof of work ,block withhold attack</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -6419,7 +6419,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>internet of things,nothing</t>
+          <t>nothing,internet of things</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -6466,7 +6466,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>bitcoin,security analysis,mine,nothing</t>
+          <t>security analysis,mine,nothing,bitcoin</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -6513,7 +6513,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>zksnarks,privacy,reward mechanism,blockchain.,bitcoin,incentive,nothing,data report,crowd-sensing,participatory sense</t>
+          <t>data report,privacy,nothing,bitcoin,blockchain.,crowd-sensing,participatory sense,reward mechanism,zksnarks,incentive</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -6560,7 +6560,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>behavior monitor,digital transaction,attack,nothing</t>
+          <t>behavior monitor,nothing,digital transaction,attack</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -6607,7 +6607,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>membership service provider,cryptographic attack,nothing</t>
+          <t>cryptographic attack,nothing,membership service provider</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -6654,7 +6654,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>decentralization,mine,reward,nothing,gap game</t>
+          <t>mine,nothing,gap game,decentralization,reward</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -6701,7 +6701,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>immutability attack,attack,nothing</t>
+          <t>immutability attack,nothing,attack</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -6748,7 +6748,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>blockmesh,compromise of the protocol,nothing</t>
+          <t>nothing,compromise of the protocol,blockmesh</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -6795,7 +6795,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>privacy,nothing</t>
+          <t>nothing,privacy</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -6842,7 +6842,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>adaptive-security,privacy,distributed-ledger,nothing,universal-composability,proof-of-stake,zero-knowledge proof</t>
+          <t>adaptive-security,universal-composability,privacy,distributed-ledger,zero-knowledge proof,nothing,proof-of-stake</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -6889,7 +6889,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>trust,nothing</t>
+          <t>nothing,trust</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -6936,7 +6936,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>intrusion detection,goldfinger attack,internet of things,statistical significance,nothing</t>
+          <t>nothing,intrusion detection,goldfinger attack,statistical significance,internet of things</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -6983,7 +6983,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>network model,consensus security,nothing</t>
+          <t>nothing,consensus security,network model</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -7030,7 +7030,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>security framework,nothing,contract,consensus protocol,threat</t>
+          <t>security framework,nothing,threat,contract,consensus protocol</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -7077,7 +7077,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>cloud compute,pool mine,data provenance,block mine,nothing,consensus protocol,blockchain security,block withhold</t>
+          <t>block mine,pool mine,nothing,blockchain security,data provenance,consensus protocol,cloud compute,block withhold</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -7124,7 +7124,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>tor,anonymity,network,cryptocurrency,bitcoin,nothing</t>
+          <t>network,tor,cryptocurrency,bitcoin,nothing,anonymity</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -7171,7 +7171,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>security vulnerability,fuzz test,system architecture,contract,nothing,ethereum</t>
+          <t>nothing,ethereum,fuzz test,security vulnerability,contract,system architecture</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -7218,7 +7218,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>cyber-physical system,nothing</t>
+          <t>nothing,cyber-physical system</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -7265,7 +7265,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>risk assessment,threat,nothing</t>
+          <t>risk assessment,nothing,threat</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -7312,7 +7312,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>performance,fork,nothing</t>
+          <t>nothing,fork,performance</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -7359,7 +7359,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>mine pool selection,evolutionary game theory,nothing,block withhold attack,consensus protocol,replicator dynamic</t>
+          <t>nothing,block withhold attack,consensus protocol,evolutionary game theory,replicator dynamic,mine pool selection</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -7406,7 +7406,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>protocol,trace analysis,triangle attack</t>
+          <t>triangle attack,trace analysis,protocol</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -7453,7 +7453,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>trust,nothing</t>
+          <t>nothing,trust</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -7500,7 +7500,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>bitcoin,cryptocurrency,privacy,nothing</t>
+          <t>nothing,bitcoin,privacy,cryptocurrency</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -7547,7 +7547,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>privacy,smart city,mobile healthcare,nothing</t>
+          <t>smart city,nothing,privacy,mobile healthcare</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -7594,7 +7594,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>privacy,industrial internet of thing privacy,industrial internet of thing security,nothing</t>
+          <t>industrial internet of thing security,nothing,industrial internet of thing privacy,privacy</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -7637,7 +7637,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>racs,nothing</t>
+          <t>nothing,racs</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -7684,7 +7684,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>attack,nothing</t>
+          <t>nothing,attack</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -7731,7 +7731,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>phishing,social engineer,malware,cryptocurrency,nothing</t>
+          <t>nothing,cryptocurrency,malware,phishing,social engineer</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -7778,7 +7778,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>immutability,logistics,network center operation,battlefield management system ,consensus protocol,nothing,defence application,peer-to-peer network ,contract,supply chain,cryptography</t>
+          <t>peer-to-peer network ,cryptography,nothing,battlefield management system ,network center operation,defence application,logistics,contract,immutability,consensus protocol,supply chain</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -7825,7 +7825,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>formal approach,theorem prove,distribute system,nothing</t>
+          <t>theorem prove,nothing,distribute system,formal approach</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -7872,7 +7872,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>cloud compute,governance,trust,law,nothing,service</t>
+          <t>governance,nothing,trust,service,cloud compute,law</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -7919,7 +7919,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>cryptography,polynomial,nothing</t>
+          <t>cryptography,nothing,polynomial</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -7966,7 +7966,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>genetic algorithm,sharding,fault tolerant,malicious attack,trust,nothing</t>
+          <t>nothing,fault tolerant,trust,malicious attack,sharding,genetic algorithm</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -8013,7 +8013,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>logic risk location,topologicalanalysis,security assurance,contract,nothing</t>
+          <t>topologicalanalysis,nothing,contract,logic risk location,security assurance</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -8060,7 +8060,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>insider threat,collaborative intrusion detection,trust management,nothing</t>
+          <t>collaborative intrusion detection,nothing,insider threat,trust management</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -8107,7 +8107,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>privacy issue,security solution,consensus protocol,security issue,privacy solution,nothing,technology</t>
+          <t>privacy solution,privacy issue,technology,nothing,security issue,consensus protocol,security solution</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -8154,7 +8154,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>wireless security,internet of things,nothing</t>
+          <t>nothing,internet of things,wireless security</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -8201,7 +8201,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>timestamp,decentralize,nothing</t>
+          <t>nothing,decentralize,timestamp</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
@@ -8248,7 +8248,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>security vulnerability,dapp,fuzz test,contract,nothing,ethereum</t>
+          <t>dapp,nothing,ethereum,fuzz test,security vulnerability,contract</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -8295,7 +8295,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>privacy,time-based zero knowledge proof of knowledge,industrial internet of thing,nothing</t>
+          <t>privacy,nothing,time-based zero knowledge proof of knowledge,industrial internet of thing</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -8342,7 +8342,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>scalability,nothing,contract,consensus protocol,test</t>
+          <t>nothing,contract,test,consensus protocol,scalability</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
@@ -8389,7 +8389,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>game,nothing</t>
+          <t>nothing,game</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -8436,7 +8436,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>proof-of-stake,attack,nothing</t>
+          <t>proof-of-stake,nothing,attack</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -8483,7 +8483,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>energy transaction,network,channel,nothing,microgrid</t>
+          <t>channel,microgrid,network,energy transaction,nothing</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
@@ -8530,7 +8530,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>internet of things,nothing</t>
+          <t>nothing,internet of things</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
@@ -8577,7 +8577,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>future scope,challenge,nothing</t>
+          <t>nothing,challenge,future scope</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -8624,7 +8624,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>integrity,security architecture,internal attack,financial system,nothing,maker-checker</t>
+          <t>nothing,integrity,security architecture,maker-checker,internal attack,financial system</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
@@ -8671,7 +8671,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>privacy,internet of things,authentication,nothing</t>
+          <t>nothing,internet of things,authentication,privacy</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -8718,7 +8718,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>program analysis,decompilation,ethereum,nothing</t>
+          <t>program analysis,nothing,decompilation,ethereum</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -8765,7 +8765,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>attack technique,dapp,contract,nothing,ethereum</t>
+          <t>dapp,nothing,ethereum,attack technique,contract</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -8812,7 +8812,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>carrier sense multiple access/collision avoidance ,network,industrial internet of thing,consensus protocol,double-spending attack,direct acyclic graph</t>
+          <t>double-spending attack,carrier sense multiple access/collision avoidance ,network,direct acyclic graph,industrial internet of thing,consensus protocol</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -8859,7 +8859,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>cybersecurity vulnerability assessment,criterion rank,nothing,cyber risk mitigation,cybersecurity framework</t>
+          <t>cybersecurity vulnerability assessment,nothing,cybersecurity framework,cyber risk mitigation,criterion rank</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -8906,7 +8906,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>sharding,failure probability,nothing,security analysis,hypergeometric distribution</t>
+          <t>failure probability,nothing,hypergeometric distribution,security analysis,sharding</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -8953,7 +8953,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>archiecture,data privacy,pki system,nothing,access control list,service</t>
+          <t>nothing,service,archiecture,access control list,data privacy,pki system</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
@@ -9000,7 +9000,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>share scheme,cryptocurrency,attack,nothing</t>
+          <t>share scheme,nothing,attack,cryptocurrency</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
@@ -9047,7 +9047,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>internet-of-things ,nothing</t>
+          <t xml:space="preserve">nothing,internet-of-things </t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -9094,7 +9094,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>cyberterrorism,cybercrime,cryptocurrency,nothing</t>
+          <t>nothing,cyberterrorism,cybercrime,cryptocurrency</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -9141,7 +9141,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>fork attack,mtc confirmation mechanism,dynamic difficulty factor,nothing</t>
+          <t>dynamic difficulty factor,nothing,mtc confirmation mechanism,fork attack</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>privacy,internet of things,iot security,nothing</t>
+          <t>nothing,internet of things,privacy,iot security</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -9235,7 +9235,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>adoption,challenge,nothing</t>
+          <t>nothing,challenge,adoption</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -9282,7 +9282,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>control,organisation.,goal,nothing</t>
+          <t>nothing,goal,control,organisation.</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -9329,7 +9329,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>,adaptive,internet of thing ,nothing</t>
+          <t>,nothing,internet of thing ,adaptive</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -9376,7 +9376,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>control,measurement,complexity,nothing</t>
+          <t>nothing,measurement,control,complexity</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
@@ -9423,7 +9423,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>privacy,application,information technology,nothing,threat</t>
+          <t>privacy,application,nothing,threat,information technology</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -9470,7 +9470,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>attack,nothing,internet of things,shv-secured hash value,cryptography,block</t>
+          <t>cryptography,attack,shv-secured hash value,nothing,block,internet of things</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -9517,7 +9517,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>risk management,stablecoin,defi,nothing</t>
+          <t>stablecoin,risk management,nothing,defi</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
@@ -9564,7 +9564,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>software lifecycle,software engineer,contract,nothing,ethereum</t>
+          <t>software engineer,nothing,ethereum,contract,software lifecycle</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -9611,7 +9611,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>solidity,contract,nothing,static analysis,vulnerability detection</t>
+          <t>solidity,vulnerability detection,nothing,contract,static analysis</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -9658,7 +9658,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>authentication,cryptocurrency,bitcoin,nothing,wallet</t>
+          <t>wallet,nothing,cryptocurrency,bitcoin,authentication</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
@@ -9705,7 +9705,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>fuzz test,machine learning,contract,nothing</t>
+          <t>fuzz test,nothing,contract,machine learning</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -9752,7 +9752,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>double-spend attack,mine,consensus protocol,nothing</t>
+          <t>double-spend attack,nothing,consensus protocol,mine</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
@@ -9799,7 +9799,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>,replay attack,security exploitation,cryptocurrency,iota,nothing</t>
+          <t>,replay attack,cryptocurrency,nothing,security exploitation,iota</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
@@ -9846,7 +9846,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>fuzzer,fuzzing,test oracle,contract,nothing,ethereum</t>
+          <t>test oracle,nothing,ethereum,fuzzing,contract,fuzzer</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
@@ -9893,7 +9893,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>solidity,fasle positive,contract,nothing,ethereum</t>
+          <t>solidity,nothing,fasle positive,ethereum,contract</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
@@ -9940,7 +9940,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>network,ethereum,eclipse-attack,nothing</t>
+          <t>nothing,eclipse-attack,ethereum,network</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
@@ -9987,7 +9987,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>ethereum,protocol,embed system,internet of things,transaction,nothing,fpga,prototype</t>
+          <t>embed system,nothing,transaction,prototype,ethereum,protocol,internet of things,fpga</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
@@ -10034,7 +10034,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>attack,real-time consensus,internet of thing ,byzantine fault-tolerant ,nothing,wireless network</t>
+          <t>internet of thing ,real-time consensus,attack,nothing,byzantine fault-tolerant ,wireless network</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
@@ -10081,7 +10081,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>emerge technology,cyber risk,risk,artificial intelligence,internet of things,nothing</t>
+          <t>emerge technology,artificial intelligence,risk,nothing,cyber risk,internet of things</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
@@ -10128,7 +10128,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>bitcoin,attack,consensus protocol,nothing</t>
+          <t>nothing,bitcoin,attack,consensus protocol</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
@@ -10175,7 +10175,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>security.,wban,nothing</t>
+          <t>nothing,wban,security.</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
@@ -10222,7 +10222,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>attack,network,consensus protocol,nothing,internet of things,contract,cryptography,hash,immutable</t>
+          <t>cryptography,hash,attack,network,nothing,contract,consensus protocol,immutable,internet of things</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
@@ -10269,7 +10269,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>openssl,fault attack,invalid curve attack,embed security,singular curve,supersingular curve</t>
+          <t>supersingular curve,openssl,embed security,fault attack,invalid curve attack,singular curve</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
@@ -10316,7 +10316,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>blockchain;-privacy,distributed-ledger,nothing,consensus protocol,hardware</t>
+          <t>blockchain;-privacy,distributed-ledger,nothing,hardware,consensus protocol</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
@@ -10363,7 +10363,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>privacy,distribute ledger technology ,internet of thing ,nothing</t>
+          <t>nothing,internet of thing ,distribute ledger technology ,privacy</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
@@ -10410,7 +10410,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t xml:space="preserve">block chain ,decentralization,peer-to-peer ,cryptocurrency,consensus protocol,nothing,cryptography,smart contract </t>
+          <t xml:space="preserve">cryptography,peer-to-peer ,nothing,cryptocurrency,smart contract ,decentralization,consensus protocol,block chain </t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
@@ -10457,7 +10457,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>censorship attack,protocol security,consensus protocol,nothing</t>
+          <t>censorship attack,nothing,protocol security,consensus protocol</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
@@ -10504,7 +10504,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>program analysis,contract,security smell,nothing</t>
+          <t>program analysis,security smell,contract,nothing</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
@@ -10551,7 +10551,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>ethereum,contract,formal approach,nothing</t>
+          <t>nothing,contract,formal approach,ethereum</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
@@ -10598,7 +10598,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>attack,interoperable-blockchains,cryptocurrency,game theory,contract,nothing,ethereum</t>
+          <t>game theory,attack,nothing,cryptocurrency,ethereum,interoperable-blockchains,contract</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
@@ -10645,7 +10645,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>spectrum sense,nothing,double threshold energy detection,ssdf attack,consensus protocol</t>
+          <t>ssdf attack,spectrum sense,nothing,double threshold energy detection,consensus protocol</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
@@ -10692,7 +10692,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>smartphone application,owasp mobile,cryptocurrency,nothing</t>
+          <t>nothing,cryptocurrency,smartphone application,owasp mobile</t>
         </is>
       </c>
       <c r="E219" t="inlineStr">
@@ -10739,7 +10739,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>contract,formal approach,nothing</t>
+          <t>nothing,contract,formal approach</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">
@@ -10786,7 +10786,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>,tangle,attack,trust,hyperledger,consensus protocol,bitcoin,ripple,contract,iota,nothing,hash,cryptography,ethereum,algor,00-01</t>
+          <t>,cryptography,hash,attack,algor,nothing,bitcoin,trust,ethereum,ripple,00-01,hyperledger,contract,consensus protocol,tangle,iota</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
@@ -10833,7 +10833,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>decentralization,security.,cryptocurrency,nothing,contract,consensus protocol,digital currency</t>
+          <t>nothing,cryptocurrency,contract,decentralization,security.,consensus protocol,digital currency</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
@@ -10880,7 +10880,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>audit log,distribute system,nothing</t>
+          <t>nothing,audit log,distribute system</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -10927,7 +10927,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>protection,input filter,contract,nothing</t>
+          <t>protection,nothing,contract,input filter</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
@@ -10974,7 +10974,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>trade-off,credit,user perception,bitcoin,nothing,debit card,usability</t>
+          <t>nothing,bitcoin,trade-off,debit card,credit,user perception,usability</t>
         </is>
       </c>
       <c r="E225" t="inlineStr">
@@ -11021,7 +11021,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>bitcoin wallet security,cryptocurrency,electrum,bitcoins,bitcoin wallet forensics,cryptocurrency wallet,multibit hd</t>
+          <t>bitcoins,multibit hd,cryptocurrency,electrum,cryptocurrency wallet,bitcoin wallet forensics,bitcoin wallet security</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
@@ -11068,7 +11068,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>risk management,internet of things,contract,financial service,practical application,technology</t>
+          <t>technology,risk management,financial service,contract,practical application,internet of things</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
@@ -11115,7 +11115,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>network,attack,consensus protocol</t>
+          <t>attack,network,consensus protocol</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
@@ -11162,7 +11162,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>attack,swift,network,payment,bank,ict,digital transaction,peer-to-peer system,nothing,financial service</t>
+          <t>attack,network,nothing,payment,digital transaction,financial service,ict,peer-to-peer system,bank,swift</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
@@ -11209,7 +11209,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>decentralize peer-to-peer,cryptocurrency,consensus protocol,bitcoin,contract,nothing,public ledger,technology</t>
+          <t>technology,cryptocurrency,nothing,bitcoin,decentralize peer-to-peer,contract,consensus protocol,public ledger</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
@@ -11256,7 +11256,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>decentralize autonomous organization,seconomics vulnerability,security protocol,fintech</t>
+          <t>decentralize autonomous organization,fintech,seconomics vulnerability,security protocol</t>
         </is>
       </c>
       <c r="E231" t="inlineStr">
@@ -11303,7 +11303,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>ethereum,contract,nothing</t>
+          <t>nothing,contract,ethereum</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
@@ -11351,7 +11351,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>internet of things,cyber physical system,contract,nothing</t>
+          <t>cyber physical system,nothing,contract,internet of things</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
@@ -11398,7 +11398,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>integrate risk analysis,nothing,ontology,reason,risk engineer</t>
+          <t>reason,integrate risk analysis,ontology,nothing,risk engineer</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
@@ -11447,7 +11447,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>vulnerability detection,contract,nothing</t>
+          <t>vulnerability detection,nothing,contract</t>
         </is>
       </c>
       <c r="E235" t="inlineStr">
@@ -11494,7 +11494,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>ethereum,propagation delay</t>
+          <t>propagation delay,ethereum</t>
         </is>
       </c>
       <c r="E236" t="inlineStr">
@@ -11541,7 +11541,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>delay,nothing,om oracle,bitcoin</t>
+          <t>om oracle,nothing,bitcoin,delay</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
@@ -11588,7 +11588,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>bitcoin,botnets,c&amp;c,nothing</t>
+          <t>nothing,bitcoin,botnets,c&amp;c</t>
         </is>
       </c>
       <c r="E238" t="inlineStr">
@@ -11635,7 +11635,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>monitor system,nothing</t>
+          <t>nothing,monitor system</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
@@ -11682,7 +11682,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>hyperledger fabric,mitigation,attack,nothing</t>
+          <t>mitigation,nothing,hyperledger fabric,attack</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
@@ -11731,7 +11731,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>p2p network,defensive protocol,bitcoin</t>
+          <t>defensive protocol,bitcoin,p2p network</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
@@ -11778,7 +11778,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>bitcoin,nothing,pay-to-public-key-hash  protocol,cryptography,trojan message attack</t>
+          <t>cryptography,nothing,bitcoin,trojan message attack,pay-to-public-key-hash  protocol</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
@@ -11825,7 +11825,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>lattice,hide number problem,ecdsa,bitcoin,crypto</t>
+          <t>lattice,ecdsa,bitcoin,crypto,hide number problem</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
@@ -11872,7 +11872,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>attack,cryptocurrency,firstcoin,nothing,consensus protocol</t>
+          <t>attack,firstcoin,nothing,cryptocurrency,consensus protocol</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
@@ -11919,7 +11919,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>banzhaf index,offline channel,collusion,nothing</t>
+          <t>collusion,nothing,offline channel,banzhaf index</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
@@ -11966,7 +11966,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>subchain,honest miner,metal node,contract,nothing</t>
+          <t>subchain,nothing,honest miner,contract,metal node</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
@@ -12013,7 +12013,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>solidity,design pattern,finite state machine,contract,nothing,ethereum,automatic code generation</t>
+          <t>solidity,design pattern,nothing,ethereum,finite state machine,contract,automatic code generation</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
@@ -12060,7 +12060,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>cryptocurrency exchange,amazon web service,cloud storage</t>
+          <t>amazon web service,cryptocurrency exchange,cloud storage</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -12107,7 +12107,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>integrity,trust,distribute immutabilization,nothing,secure log</t>
+          <t>nothing,integrity,trust,distribute immutabilization,secure log</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -12154,7 +12154,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>mine,consensus protocol,bitcoin,catalan number,nothing,dyck path,ethereum,om walk</t>
+          <t>mine,catalan number,nothing,bitcoin,dyck path,ethereum,om walk,consensus protocol</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -12201,7 +12201,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>denial of service resistance,bitcoin,consensus protocol,client puzzle,distribute computation</t>
+          <t>client puzzle,bitcoin,distribute computation,denial of service resistance,consensus protocol</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
@@ -12248,7 +12248,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>efficient storage,merkle tree,high performance compute,nothing,gpu process,consensus validation</t>
+          <t>high performance compute,nothing,gpu process,merkle tree,consensus validation,efficient storage</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
@@ -12295,7 +12295,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>privacy,cryptocurrency,threshold cryptography,bitcoin,nothing</t>
+          <t>privacy,threshold cryptography,nothing,bitcoin,cryptocurrency</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
@@ -12342,7 +12342,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>incentive compatibility,mine,bitcoin</t>
+          <t>mine,incentive compatibility,bitcoin</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
@@ -12389,7 +12389,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>solidity,contract,reentrant attack,nothing</t>
+          <t>reentrant attack,nothing,contract,solidity</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -12438,7 +12438,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>consensus protocol,softfork transition scheme,compromise hash,nothing</t>
+          <t>nothing,compromise hash,softfork transition scheme,consensus protocol</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
@@ -12485,7 +12485,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>rscoin,cryptocurrency,scalability,evaluation mechanism</t>
+          <t>scalability,cryptocurrency,rscoin,evaluation mechanism</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -12532,7 +12532,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>large deviation theory,block synchronization,game theory,correlate equilibrium</t>
+          <t>game theory,correlate equilibrium,large deviation theory,block synchronization</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
@@ -12579,7 +12579,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>data protection,decentralization,nothing</t>
+          <t>data protection,nothing,decentralization</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
@@ -12673,7 +12673,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>bitcoin security countermeasure,trend in bitcoin security breach,bitcoin</t>
+          <t>trend in bitcoin security breach,bitcoin security countermeasure,bitcoin</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
@@ -12720,7 +12720,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>challenge mechanism,fork attack,light node,binary tree,formal approach</t>
+          <t>fork attack,binary tree,light node,formal approach,challenge mechanism</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
@@ -12768,7 +12768,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>ticket owner,hyperledger fabric,invalid ticket,concert organizer,contract</t>
+          <t>hyperledger fabric,ticket owner,contract,concert organizer,invalid ticket</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
@@ -12815,7 +12815,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>security detection model,attack,mine,contrast of attack,nothing</t>
+          <t>mine,attack,nothing,security detection model,contrast of attack</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
@@ -12863,7 +12863,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>update,nothing</t>
+          <t>nothing,update</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
@@ -12910,7 +12910,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>privacy,e-cash</t>
+          <t>e-cash,privacy</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
@@ -12957,7 +12957,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>data privacy,access control encryption,decentralize sanitizers,nothing,user privacy</t>
+          <t>decentralize sanitizers,nothing,access control encryption,user privacy,data privacy</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
@@ -13005,7 +13005,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>privacy,discretionary access control,nothing</t>
+          <t>nothing,discretionary access control,privacy</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
@@ -13052,7 +13052,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>vulnerability injection,solidity,modifier issue,gas limit a a kill criterion,mutation test,contract,ethereum</t>
+          <t>solidity,mutation test,ethereum,modifier issue,gas limit a a kill criterion,contract,vulnerability injection</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
@@ -13101,7 +13101,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>human cognition,attack,cybercrime,wannacry ransomware,nothing,cyberintrusions</t>
+          <t>wannacry ransomware,cybercrime,human cognition,attack,nothing,cyberintrusions</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
@@ -13148,7 +13148,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>sleepy model,dishonest majority,bitcoin,nothing,offline player</t>
+          <t>nothing,bitcoin,dishonest majority,sleepy model,offline player</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
@@ -13195,7 +13195,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>lattice,learn with error,elliptic curve,bitcoin</t>
+          <t>elliptic curve,lattice,bitcoin,learn with error</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
@@ -13242,7 +13242,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>responsiveness,scalability,nothing,byzantine fault tolerance,cryptography</t>
+          <t>cryptography,nothing,byzantine fault tolerance,scalability,responsiveness</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -13289,7 +13289,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>game theory,mine,ddos,nothing</t>
+          <t>mine,nothing,game theory,ddos</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -13336,7 +13336,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>mine,cryptocurrency,consensus protocol,nothing</t>
+          <t>mine,nothing,consensus protocol,cryptocurrency</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -13384,7 +13384,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>intraday financial risk,garch,cryptocurrency,nothing,graph analysis</t>
+          <t>garch,graph analysis,nothing,cryptocurrency,intraday financial risk</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">

</xml_diff>